<commit_message>
check in all of the gerbers and artwork
</commit_message>
<xml_diff>
--- a/hardware/dc27_badge_kicad/BOM/bom-merged.xlsx
+++ b/hardware/dc27_badge_kicad/BOM/bom-merged.xlsx
@@ -512,9 +512,6 @@
     <t>47.5k</t>
   </si>
   <si>
-    <t>RC0201FR-0747K5L</t>
-  </si>
-  <si>
     <t>SW101</t>
   </si>
   <si>
@@ -690,6 +687,9 @@
   </si>
   <si>
     <t>MAX17055ETB+T</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF4752V</t>
   </si>
 </sst>
 </file>
@@ -2052,8 +2052,8 @@
   </sheetPr>
   <dimension ref="A1:IV114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4509,7 +4509,7 @@
         <v>130</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>162</v>
+        <v>221</v>
       </c>
       <c r="E95" s="10">
         <v>91.8</v>
@@ -4526,16 +4526,16 @@
     </row>
     <row r="96" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B96" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="C96" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C96" s="9" t="s">
+      <c r="D96" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="D96" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="E96" s="10">
         <v>111.215</v>
@@ -4552,16 +4552,16 @@
     </row>
     <row r="97" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B97" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B97" s="8" t="s">
-        <v>168</v>
-      </c>
       <c r="C97" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D97" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="D97" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="E97" s="10">
         <v>99.215000000000003</v>
@@ -4578,16 +4578,16 @@
     </row>
     <row r="98" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B98" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="B98" s="8" t="s">
-        <v>170</v>
-      </c>
       <c r="C98" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D98" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="D98" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="E98" s="10">
         <v>105.215</v>
@@ -4604,16 +4604,16 @@
     </row>
     <row r="99" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B99" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B99" s="8" t="s">
-        <v>172</v>
-      </c>
       <c r="C99" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D99" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="D99" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="E99" s="10">
         <v>105.215</v>
@@ -4630,16 +4630,16 @@
     </row>
     <row r="100" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B100" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B100" s="8" t="s">
-        <v>174</v>
-      </c>
       <c r="C100" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D100" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="D100" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="E100" s="10">
         <v>99.11</v>
@@ -4656,16 +4656,16 @@
     </row>
     <row r="101" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B101" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B101" s="8" t="s">
-        <v>176</v>
-      </c>
       <c r="C101" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D101" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="D101" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="E101" s="10">
         <v>111.11</v>
@@ -4682,16 +4682,16 @@
     </row>
     <row r="102" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B102" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B102" s="8" t="s">
-        <v>178</v>
-      </c>
       <c r="C102" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D102" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="D102" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="E102" s="10">
         <v>105.11</v>
@@ -4708,16 +4708,16 @@
     </row>
     <row r="103" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B103" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="B103" s="8" t="s">
-        <v>180</v>
-      </c>
       <c r="C103" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D103" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="D103" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="E103" s="10">
         <v>140.30000000000001</v>
@@ -4734,16 +4734,16 @@
     </row>
     <row r="104" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="C104" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C104" s="9" t="s">
+      <c r="D104" s="9" t="s">
         <v>183</v>
-      </c>
-      <c r="D104" s="9" t="s">
-        <v>184</v>
       </c>
       <c r="E104" s="10">
         <v>71</v>
@@ -4760,16 +4760,16 @@
     </row>
     <row r="105" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B105" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B105" s="8" t="s">
+      <c r="C105" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C105" s="9" t="s">
+      <c r="D105" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="D105" s="9" t="s">
-        <v>188</v>
       </c>
       <c r="E105" s="10">
         <v>129.30000000000001</v>
@@ -4786,16 +4786,16 @@
     </row>
     <row r="106" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B106" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="B106" s="8" t="s">
+      <c r="C106" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C106" s="9" t="s">
-        <v>191</v>
-      </c>
       <c r="D106" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E106" s="10">
         <v>114.62</v>
@@ -4812,16 +4812,16 @@
     </row>
     <row r="107" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B107" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="B107" s="8" t="s">
+      <c r="C107" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="C107" s="9" t="s">
+      <c r="D107" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="D107" s="9" t="s">
-        <v>195</v>
       </c>
       <c r="E107" s="10">
         <v>83.7</v>
@@ -4838,16 +4838,16 @@
     </row>
     <row r="108" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B108" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="B108" s="8" t="s">
+      <c r="C108" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="C108" s="9" t="s">
+      <c r="D108" s="9" t="s">
         <v>198</v>
-      </c>
-      <c r="D108" s="9" t="s">
-        <v>199</v>
       </c>
       <c r="E108" s="10">
         <v>85.4</v>
@@ -4864,16 +4864,16 @@
     </row>
     <row r="109" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="B109" s="8" t="s">
+      <c r="C109" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="C109" s="9" t="s">
-        <v>202</v>
-      </c>
       <c r="D109" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E109" s="10">
         <v>89.61</v>
@@ -4890,16 +4890,16 @@
     </row>
     <row r="110" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B110" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="B110" s="8" t="s">
+      <c r="C110" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C110" s="9" t="s">
-        <v>205</v>
-      </c>
       <c r="D110" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E110" s="10">
         <v>110.2</v>
@@ -4916,16 +4916,16 @@
     </row>
     <row r="111" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B111" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B111" s="8" t="s">
+      <c r="C111" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="C111" s="9" t="s">
+      <c r="D111" s="9" t="s">
         <v>208</v>
-      </c>
-      <c r="D111" s="9" t="s">
-        <v>209</v>
       </c>
       <c r="E111" s="10">
         <v>100.6</v>
@@ -4942,16 +4942,16 @@
     </row>
     <row r="112" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B112" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="B112" s="8" t="s">
+      <c r="C112" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C112" s="9" t="s">
-        <v>212</v>
-      </c>
       <c r="D112" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E112" s="10">
         <v>102.2</v>
@@ -4968,16 +4968,16 @@
     </row>
     <row r="113" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B113" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="B113" s="8" t="s">
+      <c r="C113" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="C113" s="9" t="s">
-        <v>215</v>
-      </c>
       <c r="D113" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E113" s="10">
         <v>76.510000000000005</v>
@@ -4994,16 +4994,16 @@
     </row>
     <row r="114" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B114" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="B114" s="8" t="s">
+      <c r="C114" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="C114" s="9" t="s">
+      <c r="D114" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="D114" s="9" t="s">
-        <v>219</v>
       </c>
       <c r="E114" s="10">
         <v>116.3</v>

</xml_diff>